<commit_message>
fix export medicine report
</commit_message>
<xml_diff>
--- a/Patient_Health_Management_System/wwwroot/reportTemplate/Báo cáo xuất kho thuốc.xlsx
+++ b/Patient_Health_Management_System/wwwroot/reportTemplate/Báo cáo xuất kho thuốc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anh.le5\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1fff253904016965/Documents/GitHub/Patient_Health_Management_System/Patient_Health_Management_System/wwwroot/reportTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_D23A62B3771BC41AA21427A696B8EF6751E89E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BAD6D03-EE3B-421D-8043-0C7B9C9015FA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +39,6 @@
     <t>Số lượng trong kho</t>
   </si>
   <si>
-    <t>Giá nhập</t>
-  </si>
-  <si>
-    <t>Giá bán</t>
-  </si>
-  <si>
     <t>Tên thuốc</t>
   </si>
   <si>
@@ -72,12 +67,18 @@
   </si>
   <si>
     <t>&amp;=Medicine.SellingPrice</t>
+  </si>
+  <si>
+    <t>Giá nhập (đồng)</t>
+  </si>
+  <si>
+    <t>Giá bán (đồng)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,10 +443,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -457,36 +458,36 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add import medicine via excel file
</commit_message>
<xml_diff>
--- a/Patient_Health_Management_System/wwwroot/reportTemplate/Báo cáo xuất kho thuốc.xlsx
+++ b/Patient_Health_Management_System/wwwroot/reportTemplate/Báo cáo xuất kho thuốc.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1fff253904016965/Documents/GitHub/Patient_Health_Management_System/Patient_Health_Management_System/wwwroot/reportTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_D23A62B3771BC41AA21427A696B8EF6751E89E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BAD6D03-EE3B-421D-8043-0C7B9C9015FA}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="6_{DF9B0690-0466-472B-9FB9-04C0D03490BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8905D4E-8A51-4C9E-934F-A545B4720B63}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$H$6</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID thuốc</t>
   </si>
@@ -73,13 +76,22 @@
   </si>
   <si>
     <t>Giá bán (đồng)</t>
+  </si>
+  <si>
+    <t>Báo cáo xuất kho thuốc</t>
+  </si>
+  <si>
+    <t>Thời gian:</t>
+  </si>
+  <si>
+    <t>&amp;=ExportTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,8 +107,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,9 +171,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,77 +458,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H6" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A5:H6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>